<commit_message>
add is awarded column in tender report
</commit_message>
<xml_diff>
--- a/src/private/templates/reports_tenders.xlsx
+++ b/src/private/templates/reports_tenders.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>EOI/RFQ report</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Is participated</t>
+  </si>
+  <si>
+    <t>Is awarded</t>
   </si>
 </sst>
 </file>
@@ -191,7 +194,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -500,25 +503,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1002"/>
+  <dimension ref="A1:M1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E4"/>
+      <selection activeCell="F3" sqref="F3:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.5" style="2" customWidth="1"/>
     <col min="2" max="4" width="21" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21" style="4" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" style="2" customWidth="1"/>
-    <col min="7" max="9" width="12.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.1640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="47.1640625" style="6" customWidth="1"/>
+    <col min="5" max="6" width="21" style="4" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" style="2" customWidth="1"/>
+    <col min="8" max="10" width="12.33203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.1640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="47.1640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -533,8 +536,9 @@
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
     </row>
-    <row r="2" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -547,8 +551,9 @@
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -564,145 +569,156 @@
       <c r="E3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="L3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="55" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" ht="55" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="7"/>
+      <c r="F4" s="10"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="5"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="5"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="5"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="3"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="5"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="3"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="5"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="5"/>
     </row>
-    <row r="10" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="3"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="5"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="5"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="18" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1690,20 +1706,21 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="F3:F4"/>
+  <mergeCells count="14">
     <mergeCell ref="G3:G4"/>
-    <mergeCell ref="A1:L2"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="A1:M2"/>
+    <mergeCell ref="J3:J4"/>
     <mergeCell ref="I3:I4"/>
-    <mergeCell ref="H3:H4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="D3:D4"/>
-    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="E3:E4"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>